<commit_message>
tg is done tests not passed yet!
</commit_message>
<xml_diff>
--- a/test_functions/test_exc3_pss_tg/test_for_exc3_pss_tg/exc_st3_test/res/my_Res/result_exc_st3.xlsx
+++ b/test_functions/test_exc3_pss_tg/test_for_exc3_pss_tg/exc_st3_test/res/my_Res/result_exc_st3.xlsx
@@ -44,6 +44,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -131,7 +132,7 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -184,230 +185,230 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>6.23015</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>6.3331</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>6.10252</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>6.28306</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>0.300547</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0.307944</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.297441</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.305041</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>1.87345</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1.95127</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1.81613</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1.91761</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>1.87345</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1.95127</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1.81613</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1.91761</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>0.00936726</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0.00975634</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.00908067</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.00958805</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>6.23015</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>6.3331</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>6.10252</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>6.28306</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>0.300547</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>0.307944</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>0.297441</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>0.305041</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>1.87345</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1.95127</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1.81613</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>1.91761</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>1.87345</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1.95127</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1.81613</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>1.91761</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>0.00936726</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>0.00975634</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>0.00908067</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>0.00958805</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -448,10 +449,10 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -495,7 +496,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -551,7 +552,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -607,7 +608,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -651,7 +652,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -695,7 +696,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -739,7 +740,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -780,10 +781,10 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -875,7 +876,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">

</xml_diff>